<commit_message>
Cleaned and modified Net3 Example
</commit_message>
<xml_diff>
--- a/rewet/examples/Net3/Damages/Net3-node-damage.xlsx
+++ b/rewet/examples/Net3/Damages/Net3-node-damage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snaeimi\Desktop\LADWPNET\Net3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naeim\OneDrive\Desktop\REWET\rewet\examples\Net3\Damages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EFC0FF-F788-450F-A31C-883451C8F7B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4F49C5-2BB0-4843-951D-BCF80BCC3591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{427E425A-9E87-4639-BD84-94758DCD41E1}"/>
+    <workbookView xWindow="4710" yWindow="2700" windowWidth="28800" windowHeight="15410" xr2:uid="{427E425A-9E87-4639-BD84-94758DCD41E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>node_name</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>node_Pipe_Length</t>
-  </si>
-  <si>
-    <t>node_Pre_EQ_Demand</t>
-  </si>
-  <si>
-    <t>node_Post_EQ_Demand</t>
   </si>
   <si>
     <t>time</t>
@@ -109,7 +103,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -130,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,7 +164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -276,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,21 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8759529-2512-4529-A8F3-F76DBAFD9F32}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E1" sqref="E1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -451,14 +445,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7200</v>
       </c>
@@ -471,14 +459,8 @@
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7200</v>
       </c>
@@ -491,14 +473,8 @@
       <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7200</v>
       </c>
@@ -511,14 +487,8 @@
       <c r="D4">
         <v>6.5</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7200</v>
       </c>
@@ -530,12 +500,6 @@
       </c>
       <c r="D5">
         <v>6.8</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>